<commit_message>
misc update - rename self.__player_poker_hand_management to self.__player_poker_hand_management_dict
</commit_message>
<xml_diff>
--- a/Python/source/ben/test/example-scoring.xlsx
+++ b/Python/source/ben/test/example-scoring.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
   <si>
     <t>royal flush</t>
   </si>
@@ -106,6 +106,15 @@
   </si>
   <si>
     <t>11=Jack</t>
+  </si>
+  <si>
+    <t>"as ac jd 8h 2h"</t>
+  </si>
+  <si>
+    <t>"6d 6s 10s 7c qh"</t>
+  </si>
+  <si>
+    <t>one_pair</t>
   </si>
 </sst>
 </file>
@@ -462,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q18"/>
+  <dimension ref="A1:Q22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -789,24 +798,78 @@
         <v>57</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
-        <v>26</v>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13">
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <v>1</v>
+      </c>
+      <c r="M13">
+        <v>1</v>
+      </c>
+      <c r="Q13">
+        <f>(C1*C13)+(D1*D13)+(J1*J14)+(M1*M13)</f>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" t="s">
+        <v>31</v>
+      </c>
+      <c r="H14">
+        <v>2</v>
+      </c>
+      <c r="I14">
+        <v>1</v>
+      </c>
+      <c r="L14">
+        <v>1</v>
+      </c>
+      <c r="N14">
+        <v>1</v>
+      </c>
+      <c r="Q14">
+        <f>(H1*H14)+(I1*I14)+(L1*L14)+(N1*N14)</f>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="4" t="s">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="4" t="s">
         <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D22">
+        <f>28+2+8+11</f>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>